<commit_message>
v4.8 Se actualiza el .gitignore
</commit_message>
<xml_diff>
--- a/data_clean/FENIX_ANS.xlsx
+++ b/data_clean/FENIX_ANS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hector.gaviria\Desktop\Control_ANS\data_clean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E9A7BA4-4B8C-4455-B29D-F2A0C9041846}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE7F4FD1-D5A6-4FC6-9F89-16DAB42AC8D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16214" uniqueCount="5537">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16216" uniqueCount="5540">
   <si>
     <t>PEDIDO</t>
   </si>
@@ -16647,6 +16647,15 @@
   </si>
   <si>
     <t>PENDIENTE VISITA</t>
+  </si>
+  <si>
+    <t>Validacion Sistema Fenix</t>
+  </si>
+  <si>
+    <t>SE VALIDA CONTRA EL FORMULARIO</t>
+  </si>
+  <si>
+    <t>SE VALDIA CONTAR EL EXPORTE DE CUMPLIDOS(LO FACTURADO)</t>
   </si>
 </sst>
 </file>
@@ -16665,12 +16674,14 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -16811,9 +16822,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="FENIX_ANS_TABLA" displayName="FENIX_ANS_TABLA" ref="A1:W917">
-  <autoFilter ref="A1:W917" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="FENIX_ANS_TABLA" displayName="FENIX_ANS_TABLA" ref="A1:X917">
+  <autoFilter ref="A1:X917" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="24">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="PEDIDO"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="PRODUCTO_ID"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="TIPO_TRABAJO"/>
@@ -16837,6 +16848,7 @@
     <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="DIAS_RESTANTES"/>
     <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="ESTADO"/>
     <tableColumn id="23" xr3:uid="{729A7AA8-7729-4DFB-A7FB-ECF635C8A092}" name="REPORTE FORMULARIO"/>
+    <tableColumn id="24" xr3:uid="{1525C41B-F025-44F0-8619-7B67AC1763DB}" name="Validacion Sistema Fenix"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -17127,10 +17139,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W917"/>
+  <dimension ref="A1:X917"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="S22" sqref="S22"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="X3" sqref="X3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17156,10 +17168,11 @@
     <col min="20" max="20" width="20" customWidth="1"/>
     <col min="21" max="21" width="16" customWidth="1"/>
     <col min="22" max="22" width="15" customWidth="1"/>
-    <col min="23" max="23" width="24" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="33" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="58.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -17229,8 +17242,11 @@
       <c r="W1" s="6" t="s">
         <v>5533</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X1" t="s">
+        <v>5537</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>22992467</v>
       </c>
@@ -17298,10 +17314,13 @@
         <v>36</v>
       </c>
       <c r="W2" t="s">
-        <v>5534</v>
-      </c>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+        <v>5538</v>
+      </c>
+      <c r="X2" t="s">
+        <v>5539</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>23087231</v>
       </c>
@@ -17372,7 +17391,7 @@
         <v>5535</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>23087250</v>
       </c>
@@ -17443,7 +17462,7 @@
         <v>5536</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>23087278</v>
       </c>
@@ -17514,7 +17533,7 @@
         <v>5534</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>23113448</v>
       </c>
@@ -17585,7 +17604,7 @@
         <v>5535</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>23153422</v>
       </c>
@@ -17656,7 +17675,7 @@
         <v>5535</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>23169845</v>
       </c>
@@ -17727,7 +17746,7 @@
         <v>5534</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>23201478</v>
       </c>
@@ -17795,7 +17814,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>23206334</v>
       </c>
@@ -17863,7 +17882,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>23224950</v>
       </c>
@@ -17931,7 +17950,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>23252866</v>
       </c>
@@ -17999,7 +18018,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>23252867</v>
       </c>
@@ -18067,7 +18086,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>23252885</v>
       </c>
@@ -18135,7 +18154,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>23252893</v>
       </c>
@@ -18203,7 +18222,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>23252901</v>
       </c>

</xml_diff>